<commit_message>
Fixed shooting and bullets
Player will now be shot upon when entering a guards vision. The bullet
will also reduce health. Enemy behaviour is up next.
</commit_message>
<xml_diff>
--- a/Producer Dingen/Aanwezigheid GL-G5.xlsx
+++ b/Producer Dingen/Aanwezigheid GL-G5.xlsx
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L128" sqref="L128"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,7 +1178,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="32">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B168+B160+B176</f>
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="L2" s="47">
         <f>C8+C16+C24+C32+C48+C56+C64+C72+C80+C88+C96+C104+C120+C112+C128+C136+C144+C152+C160+C168+C176</f>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="M2" s="53">
         <f>L2/K2</f>
-        <v>0.14814814814814814</v>
+        <v>0.13793103448275862</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>18</v>
@@ -1226,11 +1226,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>0.89629629629629626</v>
+        <v>0.93793103448275861</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1268,11 +1268,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.88148148148148153</v>
+        <v>0.92413793103448272</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="M5" s="56">
         <f>L5/K2</f>
-        <v>0.20370370370370369</v>
+        <v>0.18965517241379309</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>21</v>
@@ -1352,11 +1352,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.88888888888888884</v>
+        <v>0.93103448275862066</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1394,11 +1394,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.88148148148148153</v>
+        <v>0.92413793103448272</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1443,11 +1443,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.82962962962962961</v>
+        <v>0.87586206896551722</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>4.7296296296296294</v>
+        <v>4.9206896551724135</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4466,27 +4466,29 @@
       <c r="A131" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B131" s="10"/>
+      <c r="B131" s="10">
+        <v>4</v>
+      </c>
       <c r="C131" s="34">
         <v>0</v>
       </c>
       <c r="D131" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E131" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F131" s="35">
         <v>0</v>
       </c>
       <c r="G131" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H131" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I131" s="36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J131" s="2"/>
       <c r="K131" s="10"/>
@@ -4495,27 +4497,29 @@
       <c r="A132" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B132" s="10"/>
+      <c r="B132" s="10">
+        <v>6</v>
+      </c>
       <c r="C132" s="34">
         <v>0</v>
       </c>
       <c r="D132" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E132" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F132" s="35">
         <v>0</v>
       </c>
       <c r="G132" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H132" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I132" s="36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J132" s="2"/>
       <c r="K132" s="10"/>
@@ -4524,27 +4528,29 @@
       <c r="A133" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="10"/>
+      <c r="B133" s="10">
+        <v>2</v>
+      </c>
       <c r="C133" s="34">
         <v>0</v>
       </c>
       <c r="D133" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E133" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F133" s="35">
         <v>0</v>
       </c>
       <c r="G133" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H133" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I133" s="36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J133" s="2"/>
       <c r="K133" s="10"/>
@@ -4553,27 +4559,29 @@
       <c r="A134" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B134" s="10"/>
+      <c r="B134" s="10">
+        <v>4</v>
+      </c>
       <c r="C134" s="34">
         <v>0</v>
       </c>
       <c r="D134" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E134" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F134" s="35">
         <v>0</v>
       </c>
       <c r="G134" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H134" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I134" s="36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J134" s="2"/>
       <c r="K134" s="10"/>
@@ -4582,27 +4590,29 @@
       <c r="A135" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B135" s="9"/>
+      <c r="B135" s="9">
+        <v>4</v>
+      </c>
       <c r="C135" s="82">
         <v>0</v>
       </c>
       <c r="D135" s="80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E135" s="80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F135" s="80">
         <v>0</v>
       </c>
       <c r="G135" s="80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H135" s="80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I135" s="81">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J135" s="3"/>
     </row>
@@ -4611,7 +4621,7 @@
         <v>5</v>
       </c>
       <c r="B136" s="32">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C136" s="76">
         <f t="shared" ref="C136:I136" si="16">SUM(C131:C135)</f>
@@ -4619,11 +4629,11 @@
       </c>
       <c r="D136" s="77">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E136" s="77">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F136" s="77">
         <f t="shared" si="16"/>
@@ -4631,15 +4641,15 @@
       </c>
       <c r="G136" s="77">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H136" s="77">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I136" s="77">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J136" s="27"/>
       <c r="K136" s="10"/>
@@ -4673,27 +4683,29 @@
       <c r="A139" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B139" s="16"/>
+      <c r="B139" s="16">
+        <v>4</v>
+      </c>
       <c r="C139" s="34">
         <v>0</v>
       </c>
       <c r="D139" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E139" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F139" s="35">
         <v>0</v>
       </c>
       <c r="G139" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H139" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I139" s="36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J139" s="17"/>
       <c r="K139" s="10"/>
@@ -4702,27 +4714,29 @@
       <c r="A140" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B140" s="16"/>
+      <c r="B140" s="16">
+        <v>6</v>
+      </c>
       <c r="C140" s="34">
         <v>0</v>
       </c>
       <c r="D140" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E140" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F140" s="35">
         <v>0</v>
       </c>
       <c r="G140" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H140" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I140" s="36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J140" s="17"/>
       <c r="K140" s="10"/>
@@ -4731,7 +4745,9 @@
       <c r="A141" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B141" s="16"/>
+      <c r="B141" s="16">
+        <v>2</v>
+      </c>
       <c r="C141" s="34">
         <v>0</v>
       </c>
@@ -4760,7 +4776,9 @@
       <c r="A142" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B142" s="16"/>
+      <c r="B142" s="16">
+        <v>4</v>
+      </c>
       <c r="C142" s="34">
         <v>0</v>
       </c>
@@ -4789,7 +4807,9 @@
       <c r="A143" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="18"/>
+      <c r="B143" s="18">
+        <v>4</v>
+      </c>
       <c r="C143" s="82">
         <v>0</v>
       </c>
@@ -4826,11 +4846,11 @@
       </c>
       <c r="D144" s="77">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E144" s="77">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F144" s="77">
         <f t="shared" si="17"/>
@@ -4838,15 +4858,15 @@
       </c>
       <c r="G144" s="77">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H144" s="77">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I144" s="77">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J144" s="85"/>
       <c r="K144" s="10"/>

</xml_diff>

<commit_message>
Aanwezigheid, saving and loading work.
</commit_message>
<xml_diff>
--- a/Producer Dingen/Aanwezigheid GL-G5.xlsx
+++ b/Producer Dingen/Aanwezigheid GL-G5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\Documents\Important Portable Stuff V1\Year 2\Project-Ninja-Outbreak\Producer Dingen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\Desktop\Project-Ninja-Outbreak\Producer Dingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K150" sqref="K150"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,7 +1181,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="32">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B168+B160+B176</f>
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="L2" s="47">
         <f>C8+C16+C24+C32+C48+C56+C64+C72+C80+C88+C96+C104+C120+C112+C128+C136+C144+C152+C160+C168+C176</f>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="M2" s="53">
         <f>L2/K2</f>
-        <v>0.12121212121212122</v>
+        <v>0.12269938650306748</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>18</v>
@@ -1229,11 +1229,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>0.84848484848484851</v>
+        <v>0.90797546012269936</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1271,11 +1271,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.84242424242424241</v>
+        <v>0.8834355828220859</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="M5" s="56">
         <f>L5/K2</f>
-        <v>0.16666666666666666</v>
+        <v>0.16871165644171779</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>21</v>
@@ -1355,11 +1355,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.84848484848484851</v>
+        <v>0.90797546012269936</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1397,11 +1397,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.84242424242424241</v>
+        <v>0.90184049079754602</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1446,11 +1446,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I112+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.84242424242424241</v>
+        <v>0.8404907975460123</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>4.5121212121212118</v>
+        <v>4.7331288343558287</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4916,19 +4916,19 @@
         <v>0</v>
       </c>
       <c r="D147" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E147" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F147" s="35">
         <v>0</v>
       </c>
       <c r="G147" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H147" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I147" s="36">
         <v>4</v>
@@ -4947,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="D148" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E148" s="35">
         <v>0</v>
@@ -4956,10 +4956,10 @@
         <v>0</v>
       </c>
       <c r="G148" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H148" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I148" s="36">
         <v>6</v>
@@ -4978,19 +4978,19 @@
         <v>0</v>
       </c>
       <c r="D149" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E149" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F149" s="35">
         <v>0</v>
       </c>
       <c r="G149" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H149" s="35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I149" s="36">
         <v>2</v>
@@ -5009,19 +5009,19 @@
         <v>0</v>
       </c>
       <c r="D150" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E150" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F150" s="35">
         <v>0</v>
       </c>
       <c r="G150" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H150" s="35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I150" s="36">
         <v>4</v>
@@ -5034,7 +5034,7 @@
         <v>4</v>
       </c>
       <c r="B151" s="18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C151" s="82">
         <v>0</v>
@@ -5055,7 +5055,7 @@
         <v>0</v>
       </c>
       <c r="I151" s="81">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J151" s="19"/>
     </row>
@@ -5064,7 +5064,7 @@
         <v>5</v>
       </c>
       <c r="B152" s="32">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C152" s="76">
         <f t="shared" ref="C152:I152" si="18">SUM(C147:C151)</f>
@@ -5072,11 +5072,11 @@
       </c>
       <c r="D152" s="77">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E152" s="77">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F152" s="77">
         <f t="shared" si="18"/>
@@ -5084,15 +5084,15 @@
       </c>
       <c r="G152" s="77">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H152" s="77">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I152" s="77">
         <f t="shared" si="18"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J152" s="27"/>
       <c r="K152" s="10"/>

</xml_diff>